<commit_message>
Inserido dataframe e respondido 1 a 3
</commit_message>
<xml_diff>
--- a/Questões.xlsx
+++ b/Questões.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Documents\Harve - Análise de Dados\Projeto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66626289-49DA-461F-9B5F-3C82820C4031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D07837D-5AC6-43B3-807E-7E384D925F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{741F9C0B-D0D7-4906-ACDB-14FEB1C41934}"/>
   </bookViews>
@@ -27,9 +27,10 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -105,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,18 +490,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89561B21-BAFA-46ED-93F4-E98B38B35F32}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="55.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="55.296875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -511,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -522,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="20.399999999999999">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -533,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -544,7 +545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="20.399999999999999">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -555,7 +556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="20.399999999999999">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -566,7 +567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -577,7 +578,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="20.399999999999999">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -588,7 +589,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -599,7 +600,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="20.399999999999999">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -612,5 +613,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>